<commit_message>
alapoldalak + xls update
</commit_message>
<xml_diff>
--- a/szinek.xlsx
+++ b/szinek.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vagvo\Desktop\git\2023_ikt1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F72CDF-62BD-4327-B345-CBFC938F18E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D91551-F61B-4294-B1D4-CA257352C7A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Főoldal dizájnja</t>
   </si>
@@ -60,6 +60,54 @@
   </si>
   <si>
     <t>rgb(255, 255, 255)</t>
+  </si>
+  <si>
+    <t>Betűtípusok</t>
+  </si>
+  <si>
+    <t>Elem</t>
+  </si>
+  <si>
+    <t>Betűtípus</t>
+  </si>
+  <si>
+    <t>Betűstílus</t>
+  </si>
+  <si>
+    <t>Poppins</t>
+  </si>
+  <si>
+    <t>Regular 400</t>
+  </si>
+  <si>
+    <t>h1, h2, h3 címek</t>
+  </si>
+  <si>
+    <t>Regular 500</t>
+  </si>
+  <si>
+    <t>p (és minden egyéb szöveg)</t>
+  </si>
+  <si>
+    <t>navbar szövege</t>
+  </si>
+  <si>
+    <t>Open Sans</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Raleway</t>
+  </si>
+  <si>
+    <t>Fonts link</t>
+  </si>
+  <si>
+    <t>https://fonts.google.com/specimen/Raleway</t>
+  </si>
+  <si>
+    <t>https://fonts.google.com/specimen/Poppins</t>
   </si>
 </sst>
 </file>
@@ -132,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -140,6 +188,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -459,24 +508,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:D8"/>
+  <dimension ref="B2:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:5" ht="18" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -484,12 +534,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
+    <row r="6" spans="2:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -498,7 +548,7 @@
       </c>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -506,6 +556,67 @@
         <v>7</v>
       </c>
       <c r="D8" s="4"/>
+    </row>
+    <row r="11" spans="2:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="B11" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
komplex update: fooldal css fix + sajat html, css + szinek modositasa
</commit_message>
<xml_diff>
--- a/szinek.xlsx
+++ b/szinek.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vagvo\Desktop\git\2023_ikt1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C984B7A7-F637-4570-902D-48AEBFAEFFA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{852A228F-61DB-448C-9AFD-3FBDD7A20108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>Főoldal dizájnja</t>
   </si>
@@ -131,13 +131,19 @@
     <t>Betűméret</t>
   </si>
   <si>
-    <t>30px</t>
-  </si>
-  <si>
     <t>20px</t>
   </si>
   <si>
     <t>12px</t>
+  </si>
+  <si>
+    <t>55px</t>
+  </si>
+  <si>
+    <t>h1 színe</t>
+  </si>
+  <si>
+    <t>h2 színe</t>
   </si>
 </sst>
 </file>
@@ -210,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -219,6 +225,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -538,25 +545,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:E22"/>
+  <dimension ref="B2:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -564,12 +571,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -578,7 +585,7 @@
       </c>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -587,109 +594,120 @@
       </c>
       <c r="D8" s="4"/>
     </row>
-    <row r="11" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B11" s="1" t="s">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B12" s="5" t="s">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E13" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>14</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>12</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>15</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>16</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>20</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" t="s">
         <v>13</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>17</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>18</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>19</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E16" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="2:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="B17" s="1" t="s">
+    <row r="18" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B18" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B18" s="5" t="s">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C19" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>25</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" t="s">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>28</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>